<commit_message>
Edited html and example downloads
</commit_message>
<xml_diff>
--- a/src/assets/files-to-read/example_spreadsheet_small.xlsx
+++ b/src/assets/files-to-read/example_spreadsheet_small.xlsx
@@ -264,13 +264,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -293,15 +297,23 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G:G"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>